<commit_message>
Solver, devuelve equipo con formación seteada en la instancia con el mayor nivel, respetando incompatibilidades.
</commit_message>
<xml_diff>
--- a/Tp3/Jugadores.xlsx
+++ b/Tp3/Jugadores.xlsx
@@ -3,20 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IBM_ADMIN\git2\Tp3\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12060" windowHeight="5775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -175,7 +171,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -497,11 +493,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="18.140625" customWidth="1"/>
     <col min="5" max="5" width="3.28515625" customWidth="1"/>
@@ -821,7 +817,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -833,7 +829,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>